<commit_message>
dfc com o vidal cheroso
</commit_message>
<xml_diff>
--- a/Shows que já fui.xlsx
+++ b/Shows que já fui.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="180">
   <si>
     <t>Banda</t>
   </si>
@@ -552,6 +552,18 @@
   </si>
   <si>
     <t>Olho Seco</t>
+  </si>
+  <si>
+    <t>Cervical</t>
+  </si>
+  <si>
+    <t>Ataque Periférico</t>
+  </si>
+  <si>
+    <t>Revolta Civil</t>
+  </si>
+  <si>
+    <t>Heavy Duty</t>
   </si>
 </sst>
 </file>
@@ -587,7 +599,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -610,11 +622,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -656,25 +681,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -683,6 +705,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P161"/>
+  <dimension ref="A1:P165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A154" sqref="A154:A156"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,12 +1045,12 @@
       <c r="E1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="10" t="s">
         <v>71</v>
       </c>
@@ -1030,10 +1074,10 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -1045,12 +1089,12 @@
       <c r="E2" s="9">
         <v>2007</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
       <c r="J2" s="9">
         <v>2007</v>
       </c>
@@ -1060,7 +1104,7 @@
       </c>
       <c r="L2" s="9">
         <f>SUM(K2:K51)</f>
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>39</v>
@@ -1078,8 +1122,8 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="17"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1089,10 +1133,10 @@
       <c r="E3" s="7">
         <v>2007</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
       <c r="J3" s="7">
         <v>2012</v>
       </c>
@@ -1117,11 +1161,11 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="20">
         <f>(A2+1)</f>
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="20" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1133,12 +1177,12 @@
       <c r="E4" s="7">
         <v>2012</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="7">
         <v>2013</v>
       </c>
@@ -1163,8 +1207,8 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
@@ -1174,10 +1218,10 @@
       <c r="E5" s="7">
         <v>2012</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="7">
         <v>2014</v>
       </c>
@@ -1218,12 +1262,12 @@
       <c r="E6" s="7">
         <v>2012</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
       <c r="J6" s="7">
         <v>2015</v>
       </c>
@@ -1264,12 +1308,12 @@
       <c r="E7" s="7">
         <v>2013</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="7">
         <v>2016</v>
       </c>
@@ -1294,10 +1338,10 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="20">
         <v>5</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="20" t="s">
         <v>94</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -1309,12 +1353,12 @@
       <c r="E8" s="7">
         <v>2013</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
       <c r="J8" s="7">
         <v>2017</v>
       </c>
@@ -1339,8 +1383,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
@@ -1350,16 +1394,16 @@
       <c r="E9" s="7">
         <v>2013</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="7">
         <v>2018</v>
       </c>
       <c r="K9" s="7">
         <f>COUNTIF(E2:E1000,"2018")</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7" t="s">
@@ -1378,8 +1422,8 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="7" t="s">
         <v>7</v>
       </c>
@@ -1389,10 +1433,10 @@
       <c r="E10" s="7">
         <v>2013</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
@@ -1412,10 +1456,10 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="A11" s="20">
         <v>6</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="20" t="s">
         <v>116</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -1427,12 +1471,12 @@
       <c r="E11" s="7">
         <v>2013</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -1452,8 +1496,8 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1463,10 +1507,10 @@
       <c r="E12" s="7">
         <v>2013</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -1486,8 +1530,8 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1497,10 +1541,10 @@
       <c r="E13" s="7">
         <v>2013</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -1520,8 +1564,8 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="7" t="s">
         <v>12</v>
       </c>
@@ -1531,10 +1575,10 @@
       <c r="E14" s="7">
         <v>2013</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -1554,8 +1598,8 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
@@ -1565,10 +1609,10 @@
       <c r="E15" s="7">
         <v>2013</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -1588,10 +1632,10 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
+      <c r="A16" s="20">
         <v>7</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -1603,12 +1647,12 @@
       <c r="E16" s="7">
         <v>2013</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -1628,8 +1672,8 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="7" t="s">
         <v>15</v>
       </c>
@@ -1639,10 +1683,10 @@
       <c r="E17" s="7">
         <v>2013</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
@@ -1677,12 +1721,12 @@
       <c r="E18" s="7">
         <v>2014</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
@@ -1718,12 +1762,12 @@
       <c r="E19" s="7">
         <v>2014</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
@@ -1754,12 +1798,12 @@
       <c r="E20" s="7">
         <v>2014</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
@@ -1790,12 +1834,12 @@
       <c r="E21" s="7">
         <v>2014</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
@@ -1810,11 +1854,11 @@
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+      <c r="A22" s="20">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1826,12 +1870,12 @@
       <c r="E22" s="7">
         <v>2014</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
@@ -1846,8 +1890,8 @@
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="7" t="s">
         <v>97</v>
       </c>
@@ -1857,10 +1901,10 @@
       <c r="E23" s="7">
         <v>2014</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -1875,8 +1919,8 @@
       <c r="P23" s="3"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="7" t="s">
         <v>29</v>
       </c>
@@ -1886,10 +1930,10 @@
       <c r="E24" s="7">
         <v>2014</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -1919,12 +1963,12 @@
       <c r="E25" s="7">
         <v>2014</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -1939,11 +1983,11 @@
       <c r="P25" s="3"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+      <c r="A26" s="20">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="20" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1955,12 +1999,12 @@
       <c r="E26" s="7">
         <v>2014</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
@@ -1975,8 +2019,8 @@
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="7" t="s">
         <v>31</v>
       </c>
@@ -1986,10 +2030,10 @@
       <c r="E27" s="7">
         <v>2014</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
@@ -2004,10 +2048,10 @@
       <c r="P27" s="3"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
+      <c r="A28" s="20">
         <v>15</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -2019,12 +2063,12 @@
       <c r="E28" s="7">
         <v>2015</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
@@ -2039,8 +2083,8 @@
       <c r="P28" s="3"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
@@ -2050,10 +2094,10 @@
       <c r="E29" s="7">
         <v>2015</v>
       </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
@@ -2068,8 +2112,8 @@
       <c r="P29" s="3"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="7" t="s">
         <v>34</v>
       </c>
@@ -2079,10 +2123,10 @@
       <c r="E30" s="7">
         <v>2015</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
@@ -2112,12 +2156,12 @@
       <c r="E31" s="7">
         <v>2015</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
@@ -2132,11 +2176,11 @@
       <c r="P31" s="3"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
+      <c r="A32" s="20">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="22" t="s">
         <v>117</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -2148,12 +2192,12 @@
       <c r="E32" s="7">
         <v>2015</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
@@ -2168,8 +2212,8 @@
       <c r="P32" s="3"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="22"/>
       <c r="C33" s="7" t="s">
         <v>36</v>
       </c>
@@ -2179,10 +2223,10 @@
       <c r="E33" s="7">
         <v>2015</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
@@ -2197,8 +2241,8 @@
       <c r="P33" s="3"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="22"/>
       <c r="C34" s="7" t="s">
         <v>37</v>
       </c>
@@ -2208,10 +2252,10 @@
       <c r="E34" s="7">
         <v>2015</v>
       </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
@@ -2241,12 +2285,12 @@
       <c r="E35" s="7">
         <v>2015</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
@@ -2261,11 +2305,11 @@
       <c r="P35" s="3"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
+      <c r="A36" s="20">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="20" t="s">
         <v>164</v>
       </c>
       <c r="C36" s="7" t="s">
@@ -2277,12 +2321,12 @@
       <c r="E36" s="7">
         <v>2015</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
@@ -2297,8 +2341,8 @@
       <c r="P36" s="3"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="7" t="s">
         <v>39</v>
       </c>
@@ -2308,10 +2352,10 @@
       <c r="E37" s="7">
         <v>2015</v>
       </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
@@ -2326,10 +2370,10 @@
       <c r="P37" s="3"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
+      <c r="A38" s="20">
         <v>20</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="20" t="s">
         <v>116</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -2341,12 +2385,12 @@
       <c r="E38" s="7">
         <v>2015</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F38" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
@@ -2361,8 +2405,8 @@
       <c r="P38" s="3"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="7" t="s">
         <v>13</v>
       </c>
@@ -2372,10 +2416,10 @@
       <c r="E39" s="7">
         <v>2015</v>
       </c>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
       <c r="J39" s="7" t="s">
         <v>119</v>
       </c>
@@ -2392,10 +2436,10 @@
       <c r="P39" s="3"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
+      <c r="A40" s="20">
         <v>21</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="20" t="s">
         <v>116</v>
       </c>
       <c r="C40" s="7" t="s">
@@ -2407,12 +2451,12 @@
       <c r="E40" s="7">
         <v>2015</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
@@ -2427,8 +2471,8 @@
       <c r="P40" s="3"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
       <c r="C41" s="7" t="s">
         <v>161</v>
       </c>
@@ -2438,10 +2482,10 @@
       <c r="E41" s="7">
         <v>2015</v>
       </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
       <c r="L41" s="7"/>
@@ -2456,8 +2500,8 @@
       <c r="P41" s="3"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
       <c r="C42" s="7" t="s">
         <v>43</v>
       </c>
@@ -2467,10 +2511,10 @@
       <c r="E42" s="7">
         <v>2015</v>
       </c>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
       <c r="L42" s="7"/>
@@ -2485,10 +2529,10 @@
       <c r="P42" s="3"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
+      <c r="A43" s="20">
         <v>22</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="20" t="s">
         <v>116</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -2500,12 +2544,12 @@
       <c r="E43" s="7">
         <v>2015</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="F43" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
@@ -2520,8 +2564,8 @@
       <c r="P43" s="3"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
       <c r="C44" s="7" t="s">
         <v>45</v>
       </c>
@@ -2531,10 +2575,10 @@
       <c r="E44" s="7">
         <v>2015</v>
       </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
@@ -2549,8 +2593,8 @@
       <c r="P44" s="3"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
       <c r="C45" s="7" t="s">
         <v>46</v>
       </c>
@@ -2560,10 +2604,10 @@
       <c r="E45" s="7">
         <v>2015</v>
       </c>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
@@ -2578,8 +2622,8 @@
       <c r="P45" s="3"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
+      <c r="A46" s="20"/>
+      <c r="B46" s="20"/>
       <c r="C46" s="7" t="s">
         <v>47</v>
       </c>
@@ -2589,10 +2633,10 @@
       <c r="E46" s="7">
         <v>2015</v>
       </c>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
       <c r="J46" s="10" t="s">
         <v>70</v>
       </c>
@@ -2609,27 +2653,27 @@
       <c r="P46" s="3"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="17">
+      <c r="A47" s="20">
         <v>23</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D47" s="19">
+      <c r="D47" s="23">
         <v>42308</v>
       </c>
-      <c r="E47" s="17">
+      <c r="E47" s="20">
         <v>2015</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F47" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
       <c r="J47" s="7" t="s">
         <v>104</v>
       </c>
@@ -2646,15 +2690,15 @@
       <c r="P47" s="3"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
+      <c r="A48" s="20"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
       <c r="J48" s="7" t="s">
         <v>109</v>
       </c>
@@ -2671,11 +2715,11 @@
       <c r="P48" s="3"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="17">
+      <c r="A49" s="20">
         <f>(A47+1)</f>
         <v>24</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="19" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="6" t="s">
@@ -2687,12 +2731,12 @@
       <c r="E49" s="6">
         <v>2015</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="F49" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
       <c r="L49" s="7"/>
@@ -2707,8 +2751,8 @@
       <c r="P49" s="3"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="18"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="19"/>
       <c r="C50" s="6" t="s">
         <v>48</v>
       </c>
@@ -2718,10 +2762,10 @@
       <c r="E50" s="6">
         <v>2015</v>
       </c>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
@@ -2751,12 +2795,12 @@
       <c r="E51" s="6">
         <v>2015</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
       <c r="J51" s="10" t="s">
         <v>70</v>
       </c>
@@ -2789,12 +2833,12 @@
       <c r="E52" s="6">
         <v>2015</v>
       </c>
-      <c r="F52" s="17" t="s">
+      <c r="F52" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="17"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
       <c r="J52" s="7" t="s">
         <v>104</v>
       </c>
@@ -2811,28 +2855,28 @@
       <c r="P52" s="3"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" s="17">
+      <c r="A53" s="20">
         <f>(A52+1)</f>
         <v>27</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="C53" s="18" t="s">
+      <c r="C53" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D53" s="19">
+      <c r="D53" s="23">
         <v>42393</v>
       </c>
-      <c r="E53" s="18">
+      <c r="E53" s="19">
         <v>2016</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F53" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
       <c r="J53" s="7" t="s">
         <v>52</v>
       </c>
@@ -2849,15 +2893,15 @@
       <c r="P53" s="3"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
+      <c r="A54" s="20"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
       <c r="J54" s="7" t="s">
         <v>58</v>
       </c>
@@ -2874,15 +2918,15 @@
       <c r="P54" s="3"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
+      <c r="A55" s="20"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
       <c r="J55" s="7" t="s">
         <v>53</v>
       </c>
@@ -2899,15 +2943,15 @@
       <c r="P55" s="3"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
+      <c r="A56" s="20"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
       <c r="J56" s="7" t="s">
         <v>54</v>
       </c>
@@ -2924,21 +2968,21 @@
       <c r="P56" s="3"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18" t="s">
+      <c r="A57" s="20"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D57" s="19">
+      <c r="D57" s="23">
         <v>42393</v>
       </c>
-      <c r="E57" s="18">
+      <c r="E57" s="19">
         <v>2016</v>
       </c>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
       <c r="J57" s="7" t="s">
         <v>55</v>
       </c>
@@ -2955,15 +2999,15 @@
       <c r="P57" s="3"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
       <c r="J58" s="7" t="s">
         <v>56</v>
       </c>
@@ -2974,21 +3018,21 @@
       </c>
       <c r="N58" s="3">
         <f>COUNTIF(C2:C1075,"DFC")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
       <c r="J59" s="7" t="s">
         <v>57</v>
       </c>
@@ -3005,15 +3049,15 @@
       <c r="P59" s="3"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
       <c r="J60" s="7" t="s">
         <v>59</v>
       </c>
@@ -3030,11 +3074,11 @@
       <c r="P60" s="3"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="17">
+      <c r="A61" s="20">
         <f>(A53+1)</f>
         <v>28</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="19" t="s">
         <v>165</v>
       </c>
       <c r="C61" s="6" t="s">
@@ -3046,12 +3090,12 @@
       <c r="E61" s="6">
         <v>2016</v>
       </c>
-      <c r="F61" s="17" t="s">
+      <c r="F61" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
@@ -3066,8 +3110,8 @@
       <c r="P61" s="3"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
-      <c r="B62" s="18"/>
+      <c r="A62" s="20"/>
+      <c r="B62" s="19"/>
       <c r="C62" s="6" t="s">
         <v>31</v>
       </c>
@@ -3077,10 +3121,10 @@
       <c r="E62" s="6">
         <v>2016</v>
       </c>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
       <c r="L62" s="7"/>
@@ -3095,10 +3139,10 @@
       <c r="P62" s="3"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" s="17">
+      <c r="A63" s="20">
         <v>29</v>
       </c>
-      <c r="B63" s="18" t="s">
+      <c r="B63" s="19" t="s">
         <v>166</v>
       </c>
       <c r="C63" s="6" t="s">
@@ -3110,12 +3154,12 @@
       <c r="E63" s="6">
         <v>2016</v>
       </c>
-      <c r="F63" s="17" t="s">
+      <c r="F63" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
       <c r="L63" s="7"/>
@@ -3130,8 +3174,8 @@
       <c r="P63" s="3"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" s="17"/>
-      <c r="B64" s="18"/>
+      <c r="A64" s="20"/>
+      <c r="B64" s="19"/>
       <c r="C64" s="6" t="s">
         <v>62</v>
       </c>
@@ -3141,10 +3185,10 @@
       <c r="E64" s="6">
         <v>2016</v>
       </c>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="17"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
       <c r="L64" s="7"/>
@@ -3159,10 +3203,10 @@
       <c r="P64" s="3"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" s="17">
+      <c r="A65" s="20">
         <v>30</v>
       </c>
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="19" t="s">
         <v>167</v>
       </c>
       <c r="C65" s="6" t="s">
@@ -3174,12 +3218,12 @@
       <c r="E65" s="6">
         <v>2016</v>
       </c>
-      <c r="F65" s="17" t="s">
+      <c r="F65" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
       <c r="L65" s="7"/>
@@ -3189,8 +3233,8 @@
       <c r="P65" s="3"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" s="17"/>
-      <c r="B66" s="18"/>
+      <c r="A66" s="20"/>
+      <c r="B66" s="19"/>
       <c r="C66" s="6" t="s">
         <v>65</v>
       </c>
@@ -3200,10 +3244,10 @@
       <c r="E66" s="6">
         <v>2016</v>
       </c>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
       <c r="L66" s="7"/>
@@ -3228,12 +3272,12 @@
       <c r="E67" s="6">
         <v>2016</v>
       </c>
-      <c r="F67" s="17" t="s">
+      <c r="F67" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="20"/>
+      <c r="I67" s="20"/>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
       <c r="L67" s="7"/>
@@ -3243,11 +3287,11 @@
       <c r="P67" s="3"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
+      <c r="A68" s="20">
         <f t="shared" ref="A68" si="2">(A67+1)</f>
         <v>32</v>
       </c>
-      <c r="B68" s="18" t="s">
+      <c r="B68" s="19" t="s">
         <v>39</v>
       </c>
       <c r="C68" s="6" t="s">
@@ -3259,12 +3303,12 @@
       <c r="E68" s="6">
         <v>2016</v>
       </c>
-      <c r="F68" s="17" t="s">
+      <c r="F68" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="20"/>
+      <c r="I68" s="20"/>
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
       <c r="L68" s="7"/>
@@ -3274,8 +3318,8 @@
       <c r="P68" s="3"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
-      <c r="B69" s="18"/>
+      <c r="A69" s="20"/>
+      <c r="B69" s="19"/>
       <c r="C69" s="6" t="s">
         <v>73</v>
       </c>
@@ -3285,10 +3329,10 @@
       <c r="E69" s="6">
         <v>2016</v>
       </c>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
-      <c r="I69" s="17"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="20"/>
+      <c r="I69" s="20"/>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
       <c r="L69" s="7"/>
@@ -3298,8 +3342,8 @@
       <c r="P69" s="3"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70" s="17"/>
-      <c r="B70" s="18"/>
+      <c r="A70" s="20"/>
+      <c r="B70" s="19"/>
       <c r="C70" s="6" t="s">
         <v>39</v>
       </c>
@@ -3309,10 +3353,10 @@
       <c r="E70" s="6">
         <v>2016</v>
       </c>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20"/>
+      <c r="I70" s="20"/>
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
       <c r="L70" s="7"/>
@@ -3322,27 +3366,27 @@
       <c r="P70" s="3"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71" s="17">
+      <c r="A71" s="20">
         <v>33</v>
       </c>
-      <c r="B71" s="18" t="s">
+      <c r="B71" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="C71" s="18" t="s">
+      <c r="C71" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D71" s="15">
+      <c r="D71" s="18">
         <v>42588</v>
       </c>
-      <c r="E71" s="18">
+      <c r="E71" s="19">
         <v>2016</v>
       </c>
-      <c r="F71" s="14" t="s">
+      <c r="F71" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
       <c r="J71" s="10" t="s">
         <v>70</v>
       </c>
@@ -3354,15 +3398,15 @@
       <c r="P71" s="3"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
+      <c r="A72" s="20"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
+      <c r="I72" s="16"/>
       <c r="J72" s="7" t="s">
         <v>58</v>
       </c>
@@ -3374,15 +3418,15 @@
       <c r="P72" s="3"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73" s="17"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
+      <c r="A73" s="20"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
       <c r="J73" s="7" t="s">
         <v>53</v>
       </c>
@@ -3394,15 +3438,15 @@
       <c r="P73" s="3"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74" s="17"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
+      <c r="A74" s="20"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
       <c r="J74" s="7" t="s">
         <v>54</v>
       </c>
@@ -3414,15 +3458,15 @@
       <c r="P74" s="3"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A75" s="17"/>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="14"/>
+      <c r="A75" s="20"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
       <c r="J75" s="7" t="s">
         <v>80</v>
       </c>
@@ -3434,15 +3478,15 @@
       <c r="P75" s="3"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" s="17"/>
-      <c r="B76" s="18"/>
-      <c r="C76" s="18"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="14"/>
+      <c r="A76" s="20"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="16"/>
+      <c r="I76" s="16"/>
       <c r="J76" s="7" t="s">
         <v>81</v>
       </c>
@@ -3454,15 +3498,15 @@
       <c r="P76" s="3"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A77" s="17"/>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="14"/>
+      <c r="A77" s="20"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
       <c r="J77" s="7" t="s">
         <v>57</v>
       </c>
@@ -3474,15 +3518,15 @@
       <c r="P77" s="3"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A78" s="17"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="14"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="16"/>
+      <c r="I78" s="16"/>
       <c r="J78" s="7" t="s">
         <v>82</v>
       </c>
@@ -3494,15 +3538,15 @@
       <c r="P78" s="3"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A79" s="17"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="14"/>
+      <c r="A79" s="20"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="16"/>
       <c r="J79" s="7" t="s">
         <v>108</v>
       </c>
@@ -3514,15 +3558,15 @@
       <c r="P79" s="3"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A80" s="17"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="18"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="14"/>
+      <c r="A80" s="20"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="16"/>
+      <c r="I80" s="16"/>
       <c r="J80" s="6" t="s">
         <v>83</v>
       </c>
@@ -3534,28 +3578,28 @@
       <c r="P80" s="3"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A81" s="17">
+      <c r="A81" s="20">
         <f>(A71+1)</f>
         <v>34</v>
       </c>
-      <c r="B81" s="18" t="s">
+      <c r="B81" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="C81" s="18" t="s">
+      <c r="C81" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D81" s="15">
+      <c r="D81" s="18">
         <v>42589</v>
       </c>
-      <c r="E81" s="18">
+      <c r="E81" s="19">
         <v>2016</v>
       </c>
-      <c r="F81" s="14" t="s">
+      <c r="F81" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
       <c r="J81" s="10" t="s">
         <v>70</v>
       </c>
@@ -3567,15 +3611,15 @@
       <c r="P81" s="3"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A82" s="17"/>
-      <c r="B82" s="18"/>
-      <c r="C82" s="18"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="14"/>
+      <c r="A82" s="20"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
       <c r="J82" s="7" t="s">
         <v>52</v>
       </c>
@@ -3587,15 +3631,15 @@
       <c r="P82" s="3"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A83" s="17"/>
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
-      <c r="D83" s="15"/>
-      <c r="E83" s="18"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
-      <c r="I83" s="14"/>
+      <c r="A83" s="20"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="16"/>
+      <c r="I83" s="16"/>
       <c r="J83" s="7" t="s">
         <v>84</v>
       </c>
@@ -3607,15 +3651,15 @@
       <c r="P83" s="3"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A84" s="17"/>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="15"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
+      <c r="A84" s="20"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
       <c r="J84" s="7" t="s">
         <v>53</v>
       </c>
@@ -3627,15 +3671,15 @@
       <c r="P84" s="3"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A85" s="17"/>
-      <c r="B85" s="18"/>
-      <c r="C85" s="18"/>
-      <c r="D85" s="15"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="14"/>
+      <c r="A85" s="20"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
       <c r="J85" s="7" t="s">
         <v>54</v>
       </c>
@@ -3647,15 +3691,15 @@
       <c r="P85" s="3"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A86" s="17"/>
-      <c r="B86" s="18"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
+      <c r="A86" s="20"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="16"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
       <c r="J86" s="7" t="s">
         <v>90</v>
       </c>
@@ -3667,15 +3711,15 @@
       <c r="P86" s="3"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A87" s="17"/>
-      <c r="B87" s="18"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
+      <c r="A87" s="20"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="16"/>
+      <c r="I87" s="16"/>
       <c r="J87" s="7" t="s">
         <v>81</v>
       </c>
@@ -3687,15 +3731,15 @@
       <c r="P87" s="3"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A88" s="17"/>
-      <c r="B88" s="18"/>
-      <c r="C88" s="18"/>
-      <c r="D88" s="15"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
-      <c r="H88" s="14"/>
-      <c r="I88" s="14"/>
+      <c r="A88" s="20"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="16"/>
+      <c r="H88" s="16"/>
+      <c r="I88" s="16"/>
       <c r="J88" s="7" t="s">
         <v>57</v>
       </c>
@@ -3707,15 +3751,15 @@
       <c r="P88" s="3"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A89" s="17"/>
-      <c r="B89" s="18"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
+      <c r="A89" s="20"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="16"/>
+      <c r="G89" s="16"/>
+      <c r="H89" s="16"/>
+      <c r="I89" s="16"/>
       <c r="J89" s="7" t="s">
         <v>85</v>
       </c>
@@ -3727,15 +3771,15 @@
       <c r="P89" s="3"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="14"/>
+      <c r="A90" s="20"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="16"/>
+      <c r="H90" s="16"/>
+      <c r="I90" s="16"/>
       <c r="J90" s="6" t="s">
         <v>86</v>
       </c>
@@ -3747,15 +3791,15 @@
       <c r="P90" s="3"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A91" s="17"/>
-      <c r="B91" s="18"/>
-      <c r="C91" s="18"/>
-      <c r="D91" s="15"/>
-      <c r="E91" s="18"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14"/>
-      <c r="H91" s="14"/>
-      <c r="I91" s="14"/>
+      <c r="A91" s="20"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
       <c r="J91" s="6" t="s">
         <v>87</v>
       </c>
@@ -3767,15 +3811,15 @@
       <c r="P91" s="3"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A92" s="17"/>
-      <c r="B92" s="18"/>
-      <c r="C92" s="18"/>
-      <c r="D92" s="15"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="14"/>
+      <c r="A92" s="20"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
       <c r="J92" s="6" t="s">
         <v>89</v>
       </c>
@@ -3787,15 +3831,15 @@
       <c r="P92" s="3"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A93" s="17"/>
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="18"/>
-      <c r="F93" s="14"/>
-      <c r="G93" s="14"/>
-      <c r="H93" s="14"/>
-      <c r="I93" s="14"/>
+      <c r="A93" s="20"/>
+      <c r="B93" s="19"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="16"/>
+      <c r="H93" s="16"/>
+      <c r="I93" s="16"/>
       <c r="J93" s="6" t="s">
         <v>88</v>
       </c>
@@ -3807,15 +3851,15 @@
       <c r="P93" s="3"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A94" s="17"/>
-      <c r="B94" s="18"/>
-      <c r="C94" s="18"/>
-      <c r="D94" s="15"/>
-      <c r="E94" s="18"/>
-      <c r="F94" s="14"/>
-      <c r="G94" s="14"/>
-      <c r="H94" s="14"/>
-      <c r="I94" s="14"/>
+      <c r="A94" s="20"/>
+      <c r="B94" s="19"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="16"/>
+      <c r="H94" s="16"/>
+      <c r="I94" s="16"/>
       <c r="J94" s="6" t="s">
         <v>91</v>
       </c>
@@ -3827,15 +3871,15 @@
       <c r="P94" s="3"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A95" s="17"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
-      <c r="D95" s="15"/>
-      <c r="E95" s="18"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="14"/>
-      <c r="H95" s="14"/>
-      <c r="I95" s="14"/>
+      <c r="A95" s="20"/>
+      <c r="B95" s="19"/>
+      <c r="C95" s="19"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="16"/>
+      <c r="H95" s="16"/>
+      <c r="I95" s="16"/>
       <c r="J95" s="6" t="s">
         <v>92</v>
       </c>
@@ -3847,28 +3891,28 @@
       <c r="P95" s="3"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A96" s="14">
+      <c r="A96" s="16">
         <f>(A81+1)</f>
         <v>35</v>
       </c>
-      <c r="B96" s="20" t="s">
+      <c r="B96" s="25" t="s">
         <v>98</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D96" s="15">
+      <c r="D96" s="18">
         <v>42622</v>
       </c>
       <c r="E96" s="6">
         <v>2016</v>
       </c>
-      <c r="F96" s="14" t="s">
+      <c r="F96" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G96" s="14"/>
-      <c r="H96" s="14"/>
-      <c r="I96" s="14"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="16"/>
+      <c r="I96" s="16"/>
       <c r="J96" s="3"/>
       <c r="K96" s="7"/>
       <c r="L96" s="7"/>
@@ -3878,19 +3922,19 @@
       <c r="P96" s="3"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
-      <c r="B97" s="20"/>
+      <c r="A97" s="16"/>
+      <c r="B97" s="25"/>
       <c r="C97" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D97" s="14"/>
+      <c r="D97" s="16"/>
       <c r="E97" s="6">
         <v>2016</v>
       </c>
-      <c r="F97" s="14"/>
-      <c r="G97" s="14"/>
-      <c r="H97" s="14"/>
-      <c r="I97" s="14"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="16"/>
+      <c r="H97" s="16"/>
+      <c r="I97" s="16"/>
       <c r="J97" s="3"/>
       <c r="K97" s="7"/>
       <c r="L97" s="7"/>
@@ -3900,28 +3944,28 @@
       <c r="P97" s="3"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A98" s="14">
+      <c r="A98" s="16">
         <f>(A96+1)</f>
         <v>36</v>
       </c>
-      <c r="B98" s="14" t="s">
+      <c r="B98" s="16" t="s">
         <v>99</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D98" s="15">
+      <c r="D98" s="18">
         <v>42629</v>
       </c>
       <c r="E98" s="3">
         <v>2016</v>
       </c>
-      <c r="F98" s="14" t="s">
+      <c r="F98" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G98" s="14"/>
-      <c r="H98" s="14"/>
-      <c r="I98" s="14"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="16"/>
+      <c r="I98" s="16"/>
       <c r="J98" s="3"/>
       <c r="K98" s="7"/>
       <c r="L98" s="7"/>
@@ -3931,19 +3975,19 @@
       <c r="P98" s="3"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
-      <c r="B99" s="14"/>
+      <c r="A99" s="16"/>
+      <c r="B99" s="16"/>
       <c r="C99" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D99" s="15"/>
+      <c r="D99" s="18"/>
       <c r="E99" s="3">
         <v>2016</v>
       </c>
-      <c r="F99" s="14"/>
-      <c r="G99" s="14"/>
-      <c r="H99" s="14"/>
-      <c r="I99" s="14"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="16"/>
+      <c r="H99" s="16"/>
+      <c r="I99" s="16"/>
       <c r="J99" s="10" t="s">
         <v>70</v>
       </c>
@@ -3955,28 +3999,28 @@
       <c r="P99" s="3"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A100" s="14">
+      <c r="A100" s="16">
         <f>(A98+1)</f>
         <v>37</v>
       </c>
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="16" t="s">
         <v>102</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D100" s="15">
+      <c r="D100" s="18">
         <v>42637</v>
       </c>
       <c r="E100" s="3">
         <v>2016</v>
       </c>
-      <c r="F100" s="14" t="s">
+      <c r="F100" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="G100" s="14"/>
-      <c r="H100" s="14"/>
-      <c r="I100" s="14"/>
+      <c r="G100" s="16"/>
+      <c r="H100" s="16"/>
+      <c r="I100" s="16"/>
       <c r="J100" s="3" t="s">
         <v>104</v>
       </c>
@@ -3988,19 +4032,19 @@
       <c r="P100" s="3"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A101" s="14"/>
-      <c r="B101" s="14"/>
+      <c r="A101" s="16"/>
+      <c r="B101" s="16"/>
       <c r="C101" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D101" s="14"/>
+      <c r="D101" s="16"/>
       <c r="E101" s="3">
         <v>2016</v>
       </c>
-      <c r="F101" s="14"/>
-      <c r="G101" s="14"/>
-      <c r="H101" s="14"/>
-      <c r="I101" s="14"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="16"/>
+      <c r="H101" s="16"/>
+      <c r="I101" s="16"/>
       <c r="J101" s="3" t="s">
         <v>105</v>
       </c>
@@ -4012,28 +4056,28 @@
       <c r="P101" s="3"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A102" s="14">
+      <c r="A102" s="16">
         <f>(A100+1)</f>
         <v>38</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B102" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D102" s="15">
+      <c r="D102" s="18">
         <v>42643</v>
       </c>
       <c r="E102" s="3">
         <v>2016</v>
       </c>
-      <c r="F102" s="14" t="s">
+      <c r="F102" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G102" s="14"/>
-      <c r="H102" s="14"/>
-      <c r="I102" s="14"/>
+      <c r="G102" s="16"/>
+      <c r="H102" s="16"/>
+      <c r="I102" s="16"/>
       <c r="J102" s="3"/>
       <c r="K102" s="7"/>
       <c r="L102" s="7"/>
@@ -4043,19 +4087,19 @@
       <c r="P102" s="3"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
-      <c r="B103" s="14"/>
+      <c r="A103" s="16"/>
+      <c r="B103" s="16"/>
       <c r="C103" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D103" s="15"/>
+      <c r="D103" s="18"/>
       <c r="E103" s="3">
         <v>2016</v>
       </c>
-      <c r="F103" s="14"/>
-      <c r="G103" s="14"/>
-      <c r="H103" s="14"/>
-      <c r="I103" s="14"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="16"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="16"/>
       <c r="J103" s="3"/>
       <c r="K103" s="7"/>
       <c r="L103" s="7"/>
@@ -4065,19 +4109,19 @@
       <c r="P103" s="3"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
-      <c r="B104" s="14"/>
+      <c r="A104" s="16"/>
+      <c r="B104" s="16"/>
       <c r="C104" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D104" s="15"/>
+      <c r="D104" s="18"/>
       <c r="E104" s="3">
         <v>2016</v>
       </c>
-      <c r="F104" s="14"/>
-      <c r="G104" s="14"/>
-      <c r="H104" s="14"/>
-      <c r="I104" s="14"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="16"/>
+      <c r="H104" s="16"/>
+      <c r="I104" s="16"/>
       <c r="J104" s="3"/>
       <c r="K104" s="7"/>
       <c r="L104" s="7"/>
@@ -4087,28 +4131,28 @@
       <c r="P104" s="3"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A105" s="14">
+      <c r="A105" s="16">
         <f>(A102+1)</f>
         <v>39</v>
       </c>
-      <c r="B105" s="14" t="s">
+      <c r="B105" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C105" s="18" t="s">
+      <c r="C105" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D105" s="15">
+      <c r="D105" s="18">
         <v>42672</v>
       </c>
-      <c r="E105" s="16">
+      <c r="E105" s="17">
         <v>2016</v>
       </c>
-      <c r="F105" s="14" t="s">
+      <c r="F105" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G105" s="14"/>
-      <c r="H105" s="14"/>
-      <c r="I105" s="14"/>
+      <c r="G105" s="16"/>
+      <c r="H105" s="16"/>
+      <c r="I105" s="16"/>
       <c r="J105" s="10" t="s">
         <v>70</v>
       </c>
@@ -4120,15 +4164,15 @@
       <c r="P105" s="3"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="18"/>
-      <c r="D106" s="15"/>
-      <c r="E106" s="16"/>
-      <c r="F106" s="14"/>
-      <c r="G106" s="14"/>
-      <c r="H106" s="14"/>
-      <c r="I106" s="14"/>
+      <c r="A106" s="16"/>
+      <c r="B106" s="16"/>
+      <c r="C106" s="19"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="16"/>
+      <c r="H106" s="16"/>
+      <c r="I106" s="16"/>
       <c r="J106" s="7" t="s">
         <v>104</v>
       </c>
@@ -4140,15 +4184,15 @@
       <c r="P106" s="3"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A107" s="14"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="18"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="16"/>
-      <c r="F107" s="14"/>
-      <c r="G107" s="14"/>
-      <c r="H107" s="14"/>
-      <c r="I107" s="14"/>
+      <c r="A107" s="16"/>
+      <c r="B107" s="16"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="16"/>
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
       <c r="J107" s="7" t="s">
         <v>109</v>
       </c>
@@ -4160,27 +4204,27 @@
       <c r="P107" s="3"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A108" s="14">
+      <c r="A108" s="16">
         <v>40</v>
       </c>
-      <c r="B108" s="14" t="s">
+      <c r="B108" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C108" s="18" t="s">
+      <c r="C108" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D108" s="15">
+      <c r="D108" s="18">
         <v>42673</v>
       </c>
-      <c r="E108" s="16">
+      <c r="E108" s="17">
         <v>2016</v>
       </c>
-      <c r="F108" s="14" t="s">
+      <c r="F108" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G108" s="14"/>
-      <c r="H108" s="14"/>
-      <c r="I108" s="14"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="16"/>
+      <c r="I108" s="16"/>
       <c r="J108" s="10" t="s">
         <v>70</v>
       </c>
@@ -4192,15 +4236,15 @@
       <c r="P108" s="3"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A109" s="14"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="18"/>
-      <c r="D109" s="15"/>
-      <c r="E109" s="16"/>
-      <c r="F109" s="14"/>
-      <c r="G109" s="14"/>
-      <c r="H109" s="14"/>
-      <c r="I109" s="14"/>
+      <c r="A109" s="16"/>
+      <c r="B109" s="16"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="17"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="16"/>
+      <c r="I109" s="16"/>
       <c r="J109" s="7" t="s">
         <v>104</v>
       </c>
@@ -4212,8 +4256,8 @@
       <c r="P109" s="3"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A110" s="14"/>
-      <c r="B110" s="14"/>
+      <c r="A110" s="16"/>
+      <c r="B110" s="16"/>
       <c r="C110" s="6" t="s">
         <v>111</v>
       </c>
@@ -4223,10 +4267,10 @@
       <c r="E110" s="4">
         <v>2016</v>
       </c>
-      <c r="F110" s="14"/>
-      <c r="G110" s="14"/>
-      <c r="H110" s="14"/>
-      <c r="I110" s="14"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="16"/>
+      <c r="I110" s="16"/>
       <c r="J110" s="7" t="s">
         <v>112</v>
       </c>
@@ -4238,11 +4282,11 @@
       <c r="P110" s="3"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A111" s="14">
+      <c r="A111" s="16">
         <f>(A108+1)</f>
         <v>41</v>
       </c>
-      <c r="B111" s="14" t="s">
+      <c r="B111" s="16" t="s">
         <v>113</v>
       </c>
       <c r="C111" s="6" t="s">
@@ -4254,12 +4298,12 @@
       <c r="E111" s="4">
         <v>2016</v>
       </c>
-      <c r="F111" s="14" t="s">
+      <c r="F111" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G111" s="14"/>
-      <c r="H111" s="14"/>
-      <c r="I111" s="14"/>
+      <c r="G111" s="16"/>
+      <c r="H111" s="16"/>
+      <c r="I111" s="16"/>
       <c r="J111" s="10" t="s">
         <v>70</v>
       </c>
@@ -4271,8 +4315,8 @@
       <c r="P111" s="3"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A112" s="14"/>
-      <c r="B112" s="14"/>
+      <c r="A112" s="16"/>
+      <c r="B112" s="16"/>
       <c r="C112" s="6" t="s">
         <v>4</v>
       </c>
@@ -4282,10 +4326,10 @@
       <c r="E112" s="4">
         <v>2016</v>
       </c>
-      <c r="F112" s="14"/>
-      <c r="G112" s="14"/>
-      <c r="H112" s="14"/>
-      <c r="I112" s="14"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
+      <c r="I112" s="16"/>
       <c r="J112" s="7" t="s">
         <v>104</v>
       </c>
@@ -4297,11 +4341,11 @@
       <c r="P112" s="3"/>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A113" s="14">
+      <c r="A113" s="16">
         <f>(A111+1)</f>
         <v>42</v>
       </c>
-      <c r="B113" s="14" t="s">
+      <c r="B113" s="16" t="s">
         <v>113</v>
       </c>
       <c r="C113" s="6" t="s">
@@ -4313,12 +4357,12 @@
       <c r="E113" s="4">
         <v>2016</v>
       </c>
-      <c r="F113" s="14" t="s">
+      <c r="F113" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G113" s="14"/>
-      <c r="H113" s="14"/>
-      <c r="I113" s="14"/>
+      <c r="G113" s="16"/>
+      <c r="H113" s="16"/>
+      <c r="I113" s="16"/>
       <c r="J113" s="10" t="s">
         <v>70</v>
       </c>
@@ -4330,8 +4374,8 @@
       <c r="P113" s="3"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A114" s="14"/>
-      <c r="B114" s="14"/>
+      <c r="A114" s="16"/>
+      <c r="B114" s="16"/>
       <c r="C114" s="6" t="s">
         <v>39</v>
       </c>
@@ -4341,10 +4385,10 @@
       <c r="E114" s="4">
         <v>2016</v>
       </c>
-      <c r="F114" s="14"/>
-      <c r="G114" s="14"/>
-      <c r="H114" s="14"/>
-      <c r="I114" s="14"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="16"/>
+      <c r="I114" s="16"/>
       <c r="J114" s="7" t="s">
         <v>104</v>
       </c>
@@ -4372,12 +4416,12 @@
       <c r="E115" s="4">
         <v>2016</v>
       </c>
-      <c r="F115" s="14" t="s">
+      <c r="F115" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G115" s="14"/>
-      <c r="H115" s="14"/>
-      <c r="I115" s="14"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="16"/>
+      <c r="I115" s="16"/>
       <c r="J115" s="3"/>
       <c r="K115" s="7"/>
       <c r="L115" s="7"/>
@@ -4387,10 +4431,10 @@
       <c r="P115" s="3"/>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A116" s="14">
+      <c r="A116" s="16">
         <v>44</v>
       </c>
-      <c r="B116" s="14" t="s">
+      <c r="B116" s="16" t="s">
         <v>125</v>
       </c>
       <c r="C116" s="6" t="s">
@@ -4402,12 +4446,12 @@
       <c r="E116" s="4">
         <v>2016</v>
       </c>
-      <c r="F116" s="14" t="s">
+      <c r="F116" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G116" s="14"/>
-      <c r="H116" s="14"/>
-      <c r="I116" s="14"/>
+      <c r="G116" s="16"/>
+      <c r="H116" s="16"/>
+      <c r="I116" s="16"/>
       <c r="J116" s="10" t="s">
         <v>70</v>
       </c>
@@ -4419,21 +4463,21 @@
       <c r="P116" s="3"/>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A117" s="14"/>
-      <c r="B117" s="14"/>
-      <c r="C117" s="18" t="s">
+      <c r="A117" s="16"/>
+      <c r="B117" s="16"/>
+      <c r="C117" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D117" s="15">
+      <c r="D117" s="18">
         <v>42706</v>
       </c>
-      <c r="E117" s="16">
+      <c r="E117" s="17">
         <v>2016</v>
       </c>
-      <c r="F117" s="14"/>
-      <c r="G117" s="14"/>
-      <c r="H117" s="14"/>
-      <c r="I117" s="14"/>
+      <c r="F117" s="16"/>
+      <c r="G117" s="16"/>
+      <c r="H117" s="16"/>
+      <c r="I117" s="16"/>
       <c r="J117" s="7" t="s">
         <v>104</v>
       </c>
@@ -4445,15 +4489,15 @@
       <c r="P117" s="3"/>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
-      <c r="B118" s="14"/>
-      <c r="C118" s="18"/>
-      <c r="D118" s="15"/>
-      <c r="E118" s="16"/>
-      <c r="F118" s="14"/>
-      <c r="G118" s="14"/>
-      <c r="H118" s="14"/>
-      <c r="I118" s="14"/>
+      <c r="A118" s="16"/>
+      <c r="B118" s="16"/>
+      <c r="C118" s="19"/>
+      <c r="D118" s="18"/>
+      <c r="E118" s="17"/>
+      <c r="F118" s="16"/>
+      <c r="G118" s="16"/>
+      <c r="H118" s="16"/>
+      <c r="I118" s="16"/>
       <c r="J118" s="6" t="s">
         <v>121</v>
       </c>
@@ -4465,27 +4509,27 @@
       <c r="P118" s="3"/>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A119" s="14">
+      <c r="A119" s="16">
         <v>45</v>
       </c>
-      <c r="B119" s="14" t="s">
+      <c r="B119" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C119" s="18" t="s">
+      <c r="C119" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D119" s="15">
+      <c r="D119" s="18">
         <v>42718</v>
       </c>
-      <c r="E119" s="16">
+      <c r="E119" s="17">
         <v>2016</v>
       </c>
-      <c r="F119" s="14" t="s">
+      <c r="F119" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G119" s="14"/>
-      <c r="H119" s="14"/>
-      <c r="I119" s="14"/>
+      <c r="G119" s="16"/>
+      <c r="H119" s="16"/>
+      <c r="I119" s="16"/>
       <c r="J119" s="10" t="s">
         <v>70</v>
       </c>
@@ -4497,15 +4541,15 @@
       <c r="P119" s="3"/>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
-      <c r="B120" s="14"/>
-      <c r="C120" s="18"/>
-      <c r="D120" s="15"/>
-      <c r="E120" s="16"/>
-      <c r="F120" s="14"/>
-      <c r="G120" s="14"/>
-      <c r="H120" s="14"/>
-      <c r="I120" s="14"/>
+      <c r="A120" s="16"/>
+      <c r="B120" s="16"/>
+      <c r="C120" s="19"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="16"/>
+      <c r="I120" s="16"/>
       <c r="J120" s="7" t="s">
         <v>104</v>
       </c>
@@ -4517,10 +4561,10 @@
       <c r="P120" s="3"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A121" s="14">
+      <c r="A121" s="16">
         <v>46</v>
       </c>
-      <c r="B121" s="14" t="s">
+      <c r="B121" s="16" t="s">
         <v>170</v>
       </c>
       <c r="C121" s="3" t="s">
@@ -4532,12 +4576,12 @@
       <c r="E121" s="4">
         <v>2017</v>
       </c>
-      <c r="F121" s="14" t="s">
+      <c r="F121" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G121" s="14"/>
-      <c r="H121" s="14"/>
-      <c r="I121" s="14"/>
+      <c r="G121" s="16"/>
+      <c r="H121" s="16"/>
+      <c r="I121" s="16"/>
       <c r="J121" s="10" t="s">
         <v>70</v>
       </c>
@@ -4549,8 +4593,8 @@
       <c r="P121" s="3"/>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
-      <c r="B122" s="14"/>
+      <c r="A122" s="16"/>
+      <c r="B122" s="16"/>
       <c r="C122" s="3" t="s">
         <v>124</v>
       </c>
@@ -4560,10 +4604,10 @@
       <c r="E122" s="4">
         <v>2017</v>
       </c>
-      <c r="F122" s="14"/>
-      <c r="G122" s="14"/>
-      <c r="H122" s="14"/>
-      <c r="I122" s="14"/>
+      <c r="F122" s="16"/>
+      <c r="G122" s="16"/>
+      <c r="H122" s="16"/>
+      <c r="I122" s="16"/>
       <c r="J122" s="7" t="s">
         <v>104</v>
       </c>
@@ -4575,10 +4619,10 @@
       <c r="P122" s="3"/>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A123" s="14">
+      <c r="A123" s="16">
         <v>47</v>
       </c>
-      <c r="B123" s="14" t="s">
+      <c r="B123" s="16" t="s">
         <v>126</v>
       </c>
       <c r="C123" s="3" t="s">
@@ -4590,12 +4634,12 @@
       <c r="E123" s="4">
         <v>2017</v>
       </c>
-      <c r="F123" s="14" t="s">
+      <c r="F123" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="G123" s="14"/>
-      <c r="H123" s="14"/>
-      <c r="I123" s="14"/>
+      <c r="G123" s="16"/>
+      <c r="H123" s="16"/>
+      <c r="I123" s="16"/>
       <c r="J123" s="10" t="s">
         <v>70</v>
       </c>
@@ -4607,21 +4651,21 @@
       <c r="P123" s="3"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
-      <c r="B124" s="14"/>
-      <c r="C124" s="14" t="s">
+      <c r="A124" s="16"/>
+      <c r="B124" s="16"/>
+      <c r="C124" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D124" s="15">
+      <c r="D124" s="18">
         <v>42868</v>
       </c>
-      <c r="E124" s="16">
+      <c r="E124" s="17">
         <v>2017</v>
       </c>
-      <c r="F124" s="14"/>
-      <c r="G124" s="14"/>
-      <c r="H124" s="14"/>
-      <c r="I124" s="14"/>
+      <c r="F124" s="16"/>
+      <c r="G124" s="16"/>
+      <c r="H124" s="16"/>
+      <c r="I124" s="16"/>
       <c r="J124" s="9" t="s">
         <v>104</v>
       </c>
@@ -4633,15 +4677,15 @@
       <c r="P124" s="3"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
-      <c r="B125" s="14"/>
-      <c r="C125" s="14"/>
-      <c r="D125" s="15"/>
-      <c r="E125" s="16"/>
-      <c r="F125" s="14"/>
-      <c r="G125" s="14"/>
-      <c r="H125" s="14"/>
-      <c r="I125" s="14"/>
+      <c r="A125" s="16"/>
+      <c r="B125" s="16"/>
+      <c r="C125" s="16"/>
+      <c r="D125" s="18"/>
+      <c r="E125" s="17"/>
+      <c r="F125" s="16"/>
+      <c r="G125" s="16"/>
+      <c r="H125" s="16"/>
+      <c r="I125" s="16"/>
       <c r="J125" s="9" t="s">
         <v>105</v>
       </c>
@@ -4653,8 +4697,8 @@
       <c r="P125" s="3"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A126" s="14"/>
-      <c r="B126" s="14"/>
+      <c r="A126" s="16"/>
+      <c r="B126" s="16"/>
       <c r="C126" s="4" t="s">
         <v>130</v>
       </c>
@@ -4664,10 +4708,10 @@
       <c r="E126" s="4">
         <v>2017</v>
       </c>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
-      <c r="H126" s="14"/>
-      <c r="I126" s="14"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
+      <c r="H126" s="16"/>
+      <c r="I126" s="16"/>
       <c r="J126" s="9" t="s">
         <v>136</v>
       </c>
@@ -4679,8 +4723,8 @@
       <c r="P126" s="3"/>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
-      <c r="B127" s="14"/>
+      <c r="A127" s="16"/>
+      <c r="B127" s="16"/>
       <c r="C127" s="4" t="s">
         <v>11</v>
       </c>
@@ -4690,10 +4734,10 @@
       <c r="E127" s="4">
         <v>2017</v>
       </c>
-      <c r="F127" s="14"/>
-      <c r="G127" s="14"/>
-      <c r="H127" s="14"/>
-      <c r="I127" s="14"/>
+      <c r="F127" s="16"/>
+      <c r="G127" s="16"/>
+      <c r="H127" s="16"/>
+      <c r="I127" s="16"/>
       <c r="J127" s="9" t="s">
         <v>53</v>
       </c>
@@ -4705,8 +4749,8 @@
       <c r="P127" s="3"/>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A128" s="14"/>
-      <c r="B128" s="14"/>
+      <c r="A128" s="16"/>
+      <c r="B128" s="16"/>
       <c r="C128" s="4" t="s">
         <v>131</v>
       </c>
@@ -4716,10 +4760,10 @@
       <c r="E128" s="4">
         <v>2017</v>
       </c>
-      <c r="F128" s="14"/>
-      <c r="G128" s="14"/>
-      <c r="H128" s="14"/>
-      <c r="I128" s="14"/>
+      <c r="F128" s="16"/>
+      <c r="G128" s="16"/>
+      <c r="H128" s="16"/>
+      <c r="I128" s="16"/>
       <c r="J128" s="9" t="s">
         <v>137</v>
       </c>
@@ -4731,8 +4775,8 @@
       <c r="P128" s="3"/>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
-      <c r="B129" s="14"/>
+      <c r="A129" s="16"/>
+      <c r="B129" s="16"/>
       <c r="C129" s="4" t="s">
         <v>10</v>
       </c>
@@ -4742,10 +4786,10 @@
       <c r="E129" s="4">
         <v>2017</v>
       </c>
-      <c r="F129" s="14"/>
-      <c r="G129" s="14"/>
-      <c r="H129" s="14"/>
-      <c r="I129" s="14"/>
+      <c r="F129" s="16"/>
+      <c r="G129" s="16"/>
+      <c r="H129" s="16"/>
+      <c r="I129" s="16"/>
       <c r="J129" s="9" t="s">
         <v>54</v>
       </c>
@@ -4757,8 +4801,8 @@
       <c r="P129" s="3"/>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A130" s="14"/>
-      <c r="B130" s="14"/>
+      <c r="A130" s="16"/>
+      <c r="B130" s="16"/>
       <c r="C130" s="4" t="s">
         <v>132</v>
       </c>
@@ -4768,10 +4812,10 @@
       <c r="E130" s="4">
         <v>2017</v>
       </c>
-      <c r="F130" s="14"/>
-      <c r="G130" s="14"/>
-      <c r="H130" s="14"/>
-      <c r="I130" s="14"/>
+      <c r="F130" s="16"/>
+      <c r="G130" s="16"/>
+      <c r="H130" s="16"/>
+      <c r="I130" s="16"/>
       <c r="J130" s="9" t="s">
         <v>172</v>
       </c>
@@ -4783,21 +4827,21 @@
       <c r="P130" s="3"/>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A131" s="14"/>
-      <c r="B131" s="14"/>
-      <c r="C131" s="16" t="s">
+      <c r="A131" s="16"/>
+      <c r="B131" s="16"/>
+      <c r="C131" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="D131" s="15">
+      <c r="D131" s="18">
         <v>42868</v>
       </c>
-      <c r="E131" s="16">
+      <c r="E131" s="17">
         <v>2017</v>
       </c>
-      <c r="F131" s="14"/>
-      <c r="G131" s="14"/>
-      <c r="H131" s="14"/>
-      <c r="I131" s="14"/>
+      <c r="F131" s="16"/>
+      <c r="G131" s="16"/>
+      <c r="H131" s="16"/>
+      <c r="I131" s="16"/>
       <c r="J131" s="9" t="s">
         <v>57</v>
       </c>
@@ -4809,15 +4853,15 @@
       <c r="P131" s="3"/>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
-      <c r="B132" s="14"/>
-      <c r="C132" s="16"/>
-      <c r="D132" s="15"/>
-      <c r="E132" s="16"/>
-      <c r="F132" s="14"/>
-      <c r="G132" s="14"/>
-      <c r="H132" s="14"/>
-      <c r="I132" s="14"/>
+      <c r="A132" s="16"/>
+      <c r="B132" s="16"/>
+      <c r="C132" s="17"/>
+      <c r="D132" s="18"/>
+      <c r="E132" s="17"/>
+      <c r="F132" s="16"/>
+      <c r="G132" s="16"/>
+      <c r="H132" s="16"/>
+      <c r="I132" s="16"/>
       <c r="J132" s="9" t="s">
         <v>87</v>
       </c>
@@ -4829,21 +4873,21 @@
       <c r="P132" s="3"/>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
-      <c r="B133" s="14"/>
-      <c r="C133" s="16" t="s">
+      <c r="A133" s="16"/>
+      <c r="B133" s="16"/>
+      <c r="C133" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="D133" s="15">
+      <c r="D133" s="18">
         <v>42868</v>
       </c>
-      <c r="E133" s="16">
+      <c r="E133" s="17">
         <v>2017</v>
       </c>
-      <c r="F133" s="14"/>
-      <c r="G133" s="14"/>
-      <c r="H133" s="14"/>
-      <c r="I133" s="14"/>
+      <c r="F133" s="16"/>
+      <c r="G133" s="16"/>
+      <c r="H133" s="16"/>
+      <c r="I133" s="16"/>
       <c r="J133" s="9" t="s">
         <v>138</v>
       </c>
@@ -4855,15 +4899,15 @@
       <c r="P133" s="3"/>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A134" s="14"/>
-      <c r="B134" s="14"/>
-      <c r="C134" s="16"/>
-      <c r="D134" s="15"/>
-      <c r="E134" s="16"/>
-      <c r="F134" s="14"/>
-      <c r="G134" s="14"/>
-      <c r="H134" s="14"/>
-      <c r="I134" s="14"/>
+      <c r="A134" s="16"/>
+      <c r="B134" s="16"/>
+      <c r="C134" s="17"/>
+      <c r="D134" s="18"/>
+      <c r="E134" s="17"/>
+      <c r="F134" s="16"/>
+      <c r="G134" s="16"/>
+      <c r="H134" s="16"/>
+      <c r="I134" s="16"/>
       <c r="J134" s="9" t="s">
         <v>139</v>
       </c>
@@ -4875,8 +4919,8 @@
       <c r="P134" s="3"/>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A135" s="14"/>
-      <c r="B135" s="14"/>
+      <c r="A135" s="16"/>
+      <c r="B135" s="16"/>
       <c r="C135" s="4" t="s">
         <v>135</v>
       </c>
@@ -4886,10 +4930,10 @@
       <c r="E135" s="4">
         <v>2017</v>
       </c>
-      <c r="F135" s="14"/>
-      <c r="G135" s="14"/>
-      <c r="H135" s="14"/>
-      <c r="I135" s="14"/>
+      <c r="F135" s="16"/>
+      <c r="G135" s="16"/>
+      <c r="H135" s="16"/>
+      <c r="I135" s="16"/>
       <c r="J135" s="9" t="s">
         <v>140</v>
       </c>
@@ -4901,10 +4945,10 @@
       <c r="P135" s="3"/>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A136" s="14">
+      <c r="A136" s="16">
         <v>46</v>
       </c>
-      <c r="B136" s="14" t="s">
+      <c r="B136" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C136" s="4" t="s">
@@ -4916,12 +4960,12 @@
       <c r="E136" s="4">
         <v>2017</v>
       </c>
-      <c r="F136" s="14" t="s">
+      <c r="F136" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G136" s="14"/>
-      <c r="H136" s="14"/>
-      <c r="I136" s="14"/>
+      <c r="G136" s="16"/>
+      <c r="H136" s="16"/>
+      <c r="I136" s="16"/>
       <c r="J136" s="3"/>
       <c r="K136" s="3"/>
       <c r="L136" s="3"/>
@@ -4931,8 +4975,8 @@
       <c r="P136" s="3"/>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A137" s="14"/>
-      <c r="B137" s="14"/>
+      <c r="A137" s="16"/>
+      <c r="B137" s="16"/>
       <c r="C137" s="4" t="s">
         <v>143</v>
       </c>
@@ -4942,10 +4986,10 @@
       <c r="E137" s="4">
         <v>2017</v>
       </c>
-      <c r="F137" s="14"/>
-      <c r="G137" s="14"/>
-      <c r="H137" s="14"/>
-      <c r="I137" s="14"/>
+      <c r="F137" s="16"/>
+      <c r="G137" s="16"/>
+      <c r="H137" s="16"/>
+      <c r="I137" s="16"/>
       <c r="J137" s="3"/>
       <c r="K137" s="3"/>
       <c r="L137" s="3"/>
@@ -4955,8 +4999,8 @@
       <c r="P137" s="3"/>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A138" s="14"/>
-      <c r="B138" s="14"/>
+      <c r="A138" s="16"/>
+      <c r="B138" s="16"/>
       <c r="C138" s="4" t="s">
         <v>141</v>
       </c>
@@ -4966,10 +5010,10 @@
       <c r="E138" s="4">
         <v>2017</v>
       </c>
-      <c r="F138" s="14"/>
-      <c r="G138" s="14"/>
-      <c r="H138" s="14"/>
-      <c r="I138" s="14"/>
+      <c r="F138" s="16"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="16"/>
+      <c r="I138" s="16"/>
       <c r="J138" s="3"/>
       <c r="K138" s="3"/>
       <c r="L138" s="3"/>
@@ -4979,10 +5023,10 @@
       <c r="P138" s="3"/>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A139" s="14">
+      <c r="A139" s="16">
         <v>47</v>
       </c>
-      <c r="B139" s="14" t="s">
+      <c r="B139" s="16" t="s">
         <v>144</v>
       </c>
       <c r="C139" s="4" t="s">
@@ -4994,12 +5038,12 @@
       <c r="E139" s="4">
         <v>2017</v>
       </c>
-      <c r="F139" s="14" t="s">
+      <c r="F139" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G139" s="14"/>
-      <c r="H139" s="14"/>
-      <c r="I139" s="14"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="16"/>
+      <c r="I139" s="16"/>
       <c r="J139" s="3"/>
       <c r="K139" s="3"/>
       <c r="L139" s="3"/>
@@ -5009,8 +5053,8 @@
       <c r="P139" s="3"/>
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A140" s="14"/>
-      <c r="B140" s="14"/>
+      <c r="A140" s="16"/>
+      <c r="B140" s="16"/>
       <c r="C140" s="4" t="s">
         <v>146</v>
       </c>
@@ -5020,10 +5064,10 @@
       <c r="E140" s="4">
         <v>2017</v>
       </c>
-      <c r="F140" s="14"/>
-      <c r="G140" s="14"/>
-      <c r="H140" s="14"/>
-      <c r="I140" s="14"/>
+      <c r="F140" s="16"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="16"/>
+      <c r="I140" s="16"/>
       <c r="J140" s="3"/>
       <c r="K140" s="3"/>
       <c r="L140" s="3"/>
@@ -5033,8 +5077,8 @@
       <c r="P140" s="3"/>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A141" s="14"/>
-      <c r="B141" s="14"/>
+      <c r="A141" s="16"/>
+      <c r="B141" s="16"/>
       <c r="C141" s="4" t="s">
         <v>39</v>
       </c>
@@ -5044,10 +5088,10 @@
       <c r="E141" s="4">
         <v>2017</v>
       </c>
-      <c r="F141" s="14"/>
-      <c r="G141" s="14"/>
-      <c r="H141" s="14"/>
-      <c r="I141" s="14"/>
+      <c r="F141" s="16"/>
+      <c r="G141" s="16"/>
+      <c r="H141" s="16"/>
+      <c r="I141" s="16"/>
       <c r="J141" s="3"/>
       <c r="K141" s="3"/>
       <c r="L141" s="3"/>
@@ -5057,10 +5101,10 @@
       <c r="P141" s="3"/>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A142" s="14">
+      <c r="A142" s="16">
         <v>48</v>
       </c>
-      <c r="B142" s="14" t="s">
+      <c r="B142" s="16" t="s">
         <v>116</v>
       </c>
       <c r="C142" s="4" t="s">
@@ -5072,12 +5116,12 @@
       <c r="E142" s="4">
         <v>2017</v>
       </c>
-      <c r="F142" s="14" t="s">
+      <c r="F142" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="G142" s="14"/>
-      <c r="H142" s="14"/>
-      <c r="I142" s="14"/>
+      <c r="G142" s="16"/>
+      <c r="H142" s="16"/>
+      <c r="I142" s="16"/>
       <c r="J142" s="10" t="s">
         <v>70</v>
       </c>
@@ -5089,8 +5133,8 @@
       <c r="P142" s="3"/>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A143" s="14"/>
-      <c r="B143" s="14"/>
+      <c r="A143" s="16"/>
+      <c r="B143" s="16"/>
       <c r="C143" s="4" t="s">
         <v>147</v>
       </c>
@@ -5100,10 +5144,10 @@
       <c r="E143" s="4">
         <v>2017</v>
       </c>
-      <c r="F143" s="14"/>
-      <c r="G143" s="14"/>
-      <c r="H143" s="14"/>
-      <c r="I143" s="14"/>
+      <c r="F143" s="16"/>
+      <c r="G143" s="16"/>
+      <c r="H143" s="16"/>
+      <c r="I143" s="16"/>
       <c r="J143" s="7" t="s">
         <v>151</v>
       </c>
@@ -5115,8 +5159,8 @@
       <c r="P143" s="3"/>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A144" s="14"/>
-      <c r="B144" s="14"/>
+      <c r="A144" s="16"/>
+      <c r="B144" s="16"/>
       <c r="C144" s="4" t="s">
         <v>148</v>
       </c>
@@ -5126,10 +5170,10 @@
       <c r="E144" s="4">
         <v>2017</v>
       </c>
-      <c r="F144" s="14"/>
-      <c r="G144" s="14"/>
-      <c r="H144" s="14"/>
-      <c r="I144" s="14"/>
+      <c r="F144" s="16"/>
+      <c r="G144" s="16"/>
+      <c r="H144" s="16"/>
+      <c r="I144" s="16"/>
       <c r="J144" s="3"/>
       <c r="K144" s="3"/>
       <c r="L144" s="3"/>
@@ -5139,10 +5183,10 @@
       <c r="P144" s="3"/>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A145" s="14">
+      <c r="A145" s="16">
         <v>49</v>
       </c>
-      <c r="B145" s="14" t="s">
+      <c r="B145" s="16" t="s">
         <v>116</v>
       </c>
       <c r="C145" s="4" t="s">
@@ -5154,12 +5198,12 @@
       <c r="E145" s="4">
         <v>2017</v>
       </c>
-      <c r="F145" s="14" t="s">
+      <c r="F145" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="G145" s="14"/>
-      <c r="H145" s="14"/>
-      <c r="I145" s="14"/>
+      <c r="G145" s="16"/>
+      <c r="H145" s="16"/>
+      <c r="I145" s="16"/>
       <c r="J145" s="3"/>
       <c r="K145" s="3"/>
       <c r="L145" s="3"/>
@@ -5169,8 +5213,8 @@
       <c r="P145" s="3"/>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A146" s="14"/>
-      <c r="B146" s="14"/>
+      <c r="A146" s="16"/>
+      <c r="B146" s="16"/>
       <c r="C146" s="4" t="s">
         <v>149</v>
       </c>
@@ -5180,10 +5224,10 @@
       <c r="E146" s="4">
         <v>2017</v>
       </c>
-      <c r="F146" s="14"/>
-      <c r="G146" s="14"/>
-      <c r="H146" s="14"/>
-      <c r="I146" s="14"/>
+      <c r="F146" s="16"/>
+      <c r="G146" s="16"/>
+      <c r="H146" s="16"/>
+      <c r="I146" s="16"/>
       <c r="J146" s="3"/>
       <c r="K146" s="3"/>
       <c r="L146" s="3"/>
@@ -5193,8 +5237,8 @@
       <c r="P146" s="3"/>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A147" s="14"/>
-      <c r="B147" s="14"/>
+      <c r="A147" s="16"/>
+      <c r="B147" s="16"/>
       <c r="C147" s="4" t="s">
         <v>150</v>
       </c>
@@ -5204,10 +5248,10 @@
       <c r="E147" s="4">
         <v>2017</v>
       </c>
-      <c r="F147" s="14"/>
-      <c r="G147" s="14"/>
-      <c r="H147" s="14"/>
-      <c r="I147" s="14"/>
+      <c r="F147" s="16"/>
+      <c r="G147" s="16"/>
+      <c r="H147" s="16"/>
+      <c r="I147" s="16"/>
       <c r="J147" s="3"/>
       <c r="K147" s="3"/>
       <c r="L147" s="3"/>
@@ -5217,27 +5261,27 @@
       <c r="P147" s="3"/>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A148" s="17">
+      <c r="A148" s="20">
         <v>50</v>
       </c>
-      <c r="B148" s="14" t="s">
+      <c r="B148" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="C148" s="16" t="s">
+      <c r="C148" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D148" s="15">
+      <c r="D148" s="18">
         <v>43036</v>
       </c>
-      <c r="E148" s="16">
+      <c r="E148" s="17">
         <v>2017</v>
       </c>
-      <c r="F148" s="14" t="s">
+      <c r="F148" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="G148" s="14"/>
-      <c r="H148" s="14"/>
-      <c r="I148" s="14"/>
+      <c r="G148" s="16"/>
+      <c r="H148" s="16"/>
+      <c r="I148" s="16"/>
       <c r="J148" s="10" t="s">
         <v>70</v>
       </c>
@@ -5249,15 +5293,15 @@
       <c r="P148" s="3"/>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A149" s="17"/>
-      <c r="B149" s="14"/>
-      <c r="C149" s="16"/>
-      <c r="D149" s="15"/>
-      <c r="E149" s="16"/>
-      <c r="F149" s="14"/>
-      <c r="G149" s="14"/>
-      <c r="H149" s="14"/>
-      <c r="I149" s="14"/>
+      <c r="A149" s="20"/>
+      <c r="B149" s="16"/>
+      <c r="C149" s="17"/>
+      <c r="D149" s="18"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="16"/>
+      <c r="G149" s="16"/>
+      <c r="H149" s="16"/>
+      <c r="I149" s="16"/>
       <c r="J149" s="3" t="s">
         <v>87</v>
       </c>
@@ -5269,15 +5313,15 @@
       <c r="P149" s="3"/>
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A150" s="17"/>
-      <c r="B150" s="14"/>
-      <c r="C150" s="16"/>
-      <c r="D150" s="15"/>
-      <c r="E150" s="16"/>
-      <c r="F150" s="14"/>
-      <c r="G150" s="14"/>
-      <c r="H150" s="14"/>
-      <c r="I150" s="14"/>
+      <c r="A150" s="20"/>
+      <c r="B150" s="16"/>
+      <c r="C150" s="17"/>
+      <c r="D150" s="18"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="16"/>
+      <c r="G150" s="16"/>
+      <c r="H150" s="16"/>
+      <c r="I150" s="16"/>
       <c r="J150" s="3" t="s">
         <v>88</v>
       </c>
@@ -5289,15 +5333,15 @@
       <c r="P150" s="3"/>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A151" s="17"/>
-      <c r="B151" s="14"/>
-      <c r="C151" s="16"/>
-      <c r="D151" s="15"/>
-      <c r="E151" s="16"/>
-      <c r="F151" s="14"/>
-      <c r="G151" s="14"/>
-      <c r="H151" s="14"/>
-      <c r="I151" s="14"/>
+      <c r="A151" s="20"/>
+      <c r="B151" s="16"/>
+      <c r="C151" s="17"/>
+      <c r="D151" s="18"/>
+      <c r="E151" s="17"/>
+      <c r="F151" s="16"/>
+      <c r="G151" s="16"/>
+      <c r="H151" s="16"/>
+      <c r="I151" s="16"/>
       <c r="J151" s="3" t="s">
         <v>154</v>
       </c>
@@ -5309,15 +5353,15 @@
       <c r="P151" s="3"/>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A152" s="17"/>
-      <c r="B152" s="14"/>
-      <c r="C152" s="16"/>
-      <c r="D152" s="15"/>
-      <c r="E152" s="16"/>
-      <c r="F152" s="14"/>
-      <c r="G152" s="14"/>
-      <c r="H152" s="14"/>
-      <c r="I152" s="14"/>
+      <c r="A152" s="20"/>
+      <c r="B152" s="16"/>
+      <c r="C152" s="17"/>
+      <c r="D152" s="18"/>
+      <c r="E152" s="17"/>
+      <c r="F152" s="16"/>
+      <c r="G152" s="16"/>
+      <c r="H152" s="16"/>
+      <c r="I152" s="16"/>
       <c r="J152" s="3" t="s">
         <v>155</v>
       </c>
@@ -5344,12 +5388,12 @@
       <c r="E153" s="4">
         <v>2017</v>
       </c>
-      <c r="F153" s="14" t="s">
+      <c r="F153" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="G153" s="14"/>
-      <c r="H153" s="14"/>
-      <c r="I153" s="14"/>
+      <c r="G153" s="16"/>
+      <c r="H153" s="16"/>
+      <c r="I153" s="16"/>
       <c r="J153" s="3"/>
       <c r="K153" s="3"/>
       <c r="L153" s="3"/>
@@ -5359,11 +5403,11 @@
       <c r="P153" s="3"/>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A154" s="14">
+      <c r="A154" s="16">
         <f>(A153+1)</f>
         <v>52</v>
       </c>
-      <c r="B154" s="14" t="s">
+      <c r="B154" s="16" t="s">
         <v>160</v>
       </c>
       <c r="C154" s="3" t="s">
@@ -5375,12 +5419,12 @@
       <c r="E154" s="4">
         <v>2018</v>
       </c>
-      <c r="F154" s="14" t="s">
+      <c r="F154" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G154" s="14"/>
-      <c r="H154" s="14"/>
-      <c r="I154" s="14"/>
+      <c r="G154" s="16"/>
+      <c r="H154" s="16"/>
+      <c r="I154" s="16"/>
       <c r="J154" s="9"/>
       <c r="K154" s="3"/>
       <c r="L154" s="3"/>
@@ -5390,8 +5434,8 @@
       <c r="P154" s="3"/>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A155" s="14"/>
-      <c r="B155" s="14"/>
+      <c r="A155" s="16"/>
+      <c r="B155" s="16"/>
       <c r="C155" s="4" t="s">
         <v>161</v>
       </c>
@@ -5401,10 +5445,10 @@
       <c r="E155" s="4">
         <v>2018</v>
       </c>
-      <c r="F155" s="14"/>
-      <c r="G155" s="14"/>
-      <c r="H155" s="14"/>
-      <c r="I155" s="14"/>
+      <c r="F155" s="16"/>
+      <c r="G155" s="16"/>
+      <c r="H155" s="16"/>
+      <c r="I155" s="16"/>
       <c r="J155" s="2"/>
       <c r="K155" s="3"/>
       <c r="L155" s="3"/>
@@ -5414,8 +5458,8 @@
       <c r="P155" s="3"/>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A156" s="14"/>
-      <c r="B156" s="14"/>
+      <c r="A156" s="16"/>
+      <c r="B156" s="16"/>
       <c r="C156" s="4" t="s">
         <v>34</v>
       </c>
@@ -5425,10 +5469,10 @@
       <c r="E156" s="4">
         <v>2018</v>
       </c>
-      <c r="F156" s="14"/>
-      <c r="G156" s="14"/>
-      <c r="H156" s="14"/>
-      <c r="I156" s="14"/>
+      <c r="F156" s="16"/>
+      <c r="G156" s="16"/>
+      <c r="H156" s="16"/>
+      <c r="I156" s="16"/>
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
       <c r="L156" s="3"/>
@@ -5453,12 +5497,12 @@
       <c r="E157" s="4">
         <v>2018</v>
       </c>
-      <c r="F157" s="14" t="s">
+      <c r="F157" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="G157" s="14"/>
-      <c r="H157" s="14"/>
-      <c r="I157" s="14"/>
+      <c r="G157" s="16"/>
+      <c r="H157" s="16"/>
+      <c r="I157" s="16"/>
       <c r="J157" s="3"/>
       <c r="K157" s="3"/>
       <c r="L157" s="3"/>
@@ -5468,10 +5512,10 @@
       <c r="P157" s="3"/>
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A158" s="14">
+      <c r="A158" s="16">
         <v>54</v>
       </c>
-      <c r="B158" s="14" t="s">
+      <c r="B158" s="16" t="s">
         <v>144</v>
       </c>
       <c r="C158" s="12" t="s">
@@ -5483,16 +5527,16 @@
       <c r="E158" s="12">
         <v>2018</v>
       </c>
-      <c r="F158" s="14" t="s">
+      <c r="F158" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G158" s="14"/>
-      <c r="H158" s="14"/>
-      <c r="I158" s="14"/>
+      <c r="G158" s="16"/>
+      <c r="H158" s="16"/>
+      <c r="I158" s="16"/>
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A159" s="14"/>
-      <c r="B159" s="14"/>
+      <c r="A159" s="16"/>
+      <c r="B159" s="16"/>
       <c r="C159" s="12" t="s">
         <v>174</v>
       </c>
@@ -5502,14 +5546,14 @@
       <c r="E159" s="11">
         <v>2018</v>
       </c>
-      <c r="F159" s="14"/>
-      <c r="G159" s="14"/>
-      <c r="H159" s="14"/>
-      <c r="I159" s="14"/>
+      <c r="F159" s="16"/>
+      <c r="G159" s="16"/>
+      <c r="H159" s="16"/>
+      <c r="I159" s="16"/>
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A160" s="14"/>
-      <c r="B160" s="14"/>
+      <c r="A160" s="16"/>
+      <c r="B160" s="16"/>
       <c r="C160" s="12" t="s">
         <v>175</v>
       </c>
@@ -5519,33 +5563,278 @@
       <c r="E160" s="11">
         <v>2018</v>
       </c>
-      <c r="F160" s="14"/>
-      <c r="G160" s="14"/>
-      <c r="H160" s="14"/>
-      <c r="I160" s="14"/>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A161" s="14"/>
-      <c r="B161" s="14"/>
-      <c r="C161" s="12" t="s">
+      <c r="F160" s="16"/>
+      <c r="G160" s="16"/>
+      <c r="H160" s="16"/>
+      <c r="I160" s="16"/>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" s="26"/>
+      <c r="B161" s="26"/>
+      <c r="C161" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D161" s="13">
+      <c r="D161" s="28">
         <v>43309</v>
       </c>
-      <c r="E161" s="11">
+      <c r="E161" s="29">
         <v>2018</v>
       </c>
-      <c r="F161" s="14"/>
-      <c r="G161" s="14"/>
-      <c r="H161" s="14"/>
-      <c r="I161" s="14"/>
+      <c r="F161" s="26"/>
+      <c r="G161" s="26"/>
+      <c r="H161" s="26"/>
+      <c r="I161" s="26"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" s="16">
+        <v>55</v>
+      </c>
+      <c r="B162" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C162" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D162" s="30">
+        <v>43330</v>
+      </c>
+      <c r="E162" s="14">
+        <v>2018</v>
+      </c>
+      <c r="F162" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="G162" s="16"/>
+      <c r="H162" s="16"/>
+      <c r="I162" s="16"/>
+      <c r="J162" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" s="16"/>
+      <c r="B163" s="16"/>
+      <c r="C163" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D163" s="30">
+        <v>43330</v>
+      </c>
+      <c r="E163" s="14">
+        <v>2018</v>
+      </c>
+      <c r="F163" s="16"/>
+      <c r="G163" s="16"/>
+      <c r="H163" s="16"/>
+      <c r="I163" s="16"/>
+      <c r="J163" s="24"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" s="16"/>
+      <c r="B164" s="16"/>
+      <c r="C164" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D164" s="30">
+        <v>43330</v>
+      </c>
+      <c r="E164" s="14">
+        <v>2018</v>
+      </c>
+      <c r="F164" s="16"/>
+      <c r="G164" s="16"/>
+      <c r="H164" s="16"/>
+      <c r="I164" s="16"/>
+      <c r="J164" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165" s="16"/>
+      <c r="B165" s="16"/>
+      <c r="C165" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D165" s="30">
+        <v>43330</v>
+      </c>
+      <c r="E165" s="14">
+        <v>2018</v>
+      </c>
+      <c r="F165" s="16"/>
+      <c r="G165" s="16"/>
+      <c r="H165" s="16"/>
+      <c r="I165" s="16"/>
+      <c r="J165" s="16"/>
     </row>
   </sheetData>
   <sortState ref="M3:N51">
     <sortCondition descending="1" ref="N3:N51"/>
   </sortState>
-  <mergeCells count="182">
+  <mergeCells count="187">
+    <mergeCell ref="B162:B165"/>
+    <mergeCell ref="A162:A165"/>
+    <mergeCell ref="F162:I165"/>
+    <mergeCell ref="J164:J165"/>
+    <mergeCell ref="J162:J163"/>
+    <mergeCell ref="F157:I157"/>
+    <mergeCell ref="F153:I153"/>
+    <mergeCell ref="A139:A141"/>
+    <mergeCell ref="A142:A144"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="B139:B141"/>
+    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="B145:B147"/>
+    <mergeCell ref="F139:I141"/>
+    <mergeCell ref="F142:I144"/>
+    <mergeCell ref="F145:I147"/>
+    <mergeCell ref="F148:I152"/>
+    <mergeCell ref="D148:D152"/>
+    <mergeCell ref="E148:E152"/>
+    <mergeCell ref="C148:C152"/>
+    <mergeCell ref="B148:B152"/>
+    <mergeCell ref="A148:A152"/>
+    <mergeCell ref="F154:I156"/>
+    <mergeCell ref="B154:B156"/>
+    <mergeCell ref="A154:A156"/>
+    <mergeCell ref="F123:I135"/>
+    <mergeCell ref="B123:B135"/>
+    <mergeCell ref="A123:A135"/>
+    <mergeCell ref="C133:C134"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="D133:D134"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="E131:E132"/>
+    <mergeCell ref="E133:E134"/>
+    <mergeCell ref="F116:I118"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="E117:E118"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="A116:A118"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="F98:I99"/>
+    <mergeCell ref="F68:I70"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:I110"/>
+    <mergeCell ref="F102:I104"/>
+    <mergeCell ref="C81:C95"/>
+    <mergeCell ref="D81:D95"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="B105:B107"/>
+    <mergeCell ref="C105:C107"/>
+    <mergeCell ref="D105:D107"/>
+    <mergeCell ref="E105:E107"/>
+    <mergeCell ref="F105:I107"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="F28:I30"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="E53:E56"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B53:B60"/>
+    <mergeCell ref="A81:A95"/>
+    <mergeCell ref="F49:I50"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B71:B80"/>
+    <mergeCell ref="B81:B95"/>
+    <mergeCell ref="F63:I64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="F53:I60"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A53:A60"/>
+    <mergeCell ref="F47:I48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="F32:I34"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F36:I37"/>
+    <mergeCell ref="F38:I39"/>
+    <mergeCell ref="F40:I42"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="F16:I17"/>
+    <mergeCell ref="F22:I24"/>
+    <mergeCell ref="F26:I27"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F43:I46"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F96:I97"/>
+    <mergeCell ref="F2:I3"/>
+    <mergeCell ref="F4:I5"/>
+    <mergeCell ref="F8:I10"/>
+    <mergeCell ref="F11:I15"/>
+    <mergeCell ref="F111:I112"/>
+    <mergeCell ref="F113:I114"/>
+    <mergeCell ref="B102:B104"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="F100:I101"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F65:I66"/>
+    <mergeCell ref="F61:I62"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="E81:E95"/>
+    <mergeCell ref="F81:I95"/>
+    <mergeCell ref="F71:I80"/>
+    <mergeCell ref="E71:E80"/>
+    <mergeCell ref="D71:D80"/>
+    <mergeCell ref="C71:C80"/>
+    <mergeCell ref="A71:A80"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B65:B66"/>
     <mergeCell ref="F158:I161"/>
     <mergeCell ref="B158:B161"/>
     <mergeCell ref="A158:A161"/>
@@ -5570,164 +5859,6 @@
     <mergeCell ref="A111:A112"/>
     <mergeCell ref="A113:A114"/>
     <mergeCell ref="B113:B114"/>
-    <mergeCell ref="E81:E95"/>
-    <mergeCell ref="F81:I95"/>
-    <mergeCell ref="F71:I80"/>
-    <mergeCell ref="E71:E80"/>
-    <mergeCell ref="D71:D80"/>
-    <mergeCell ref="C71:C80"/>
-    <mergeCell ref="A71:A80"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="F96:I97"/>
-    <mergeCell ref="F2:I3"/>
-    <mergeCell ref="F4:I5"/>
-    <mergeCell ref="F8:I10"/>
-    <mergeCell ref="F11:I15"/>
-    <mergeCell ref="F111:I112"/>
-    <mergeCell ref="F113:I114"/>
-    <mergeCell ref="B102:B104"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="D100:D101"/>
-    <mergeCell ref="F100:I101"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F65:I66"/>
-    <mergeCell ref="F61:I62"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="F32:I34"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F36:I37"/>
-    <mergeCell ref="F38:I39"/>
-    <mergeCell ref="F40:I42"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="F16:I17"/>
-    <mergeCell ref="F22:I24"/>
-    <mergeCell ref="F26:I27"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F43:I46"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="F53:I60"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="F47:I48"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="F28:I30"/>
-    <mergeCell ref="C57:C60"/>
-    <mergeCell ref="C53:C56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="E53:E56"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B53:B60"/>
-    <mergeCell ref="A81:A95"/>
-    <mergeCell ref="F49:I50"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="B71:B80"/>
-    <mergeCell ref="B81:B95"/>
-    <mergeCell ref="F63:I64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="F116:I118"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="D117:D118"/>
-    <mergeCell ref="E117:E118"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="A116:A118"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="F98:I99"/>
-    <mergeCell ref="F68:I70"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:I110"/>
-    <mergeCell ref="F102:I104"/>
-    <mergeCell ref="C81:C95"/>
-    <mergeCell ref="D81:D95"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="B105:B107"/>
-    <mergeCell ref="C105:C107"/>
-    <mergeCell ref="D105:D107"/>
-    <mergeCell ref="E105:E107"/>
-    <mergeCell ref="F105:I107"/>
-    <mergeCell ref="F123:I135"/>
-    <mergeCell ref="B123:B135"/>
-    <mergeCell ref="A123:A135"/>
-    <mergeCell ref="C133:C134"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="D124:D125"/>
-    <mergeCell ref="D131:D132"/>
-    <mergeCell ref="D133:D134"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="E131:E132"/>
-    <mergeCell ref="E133:E134"/>
-    <mergeCell ref="F157:I157"/>
-    <mergeCell ref="F153:I153"/>
-    <mergeCell ref="A139:A141"/>
-    <mergeCell ref="A142:A144"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="B139:B141"/>
-    <mergeCell ref="B142:B144"/>
-    <mergeCell ref="B145:B147"/>
-    <mergeCell ref="F139:I141"/>
-    <mergeCell ref="F142:I144"/>
-    <mergeCell ref="F145:I147"/>
-    <mergeCell ref="F148:I152"/>
-    <mergeCell ref="D148:D152"/>
-    <mergeCell ref="E148:E152"/>
-    <mergeCell ref="C148:C152"/>
-    <mergeCell ref="B148:B152"/>
-    <mergeCell ref="A148:A152"/>
-    <mergeCell ref="F154:I156"/>
-    <mergeCell ref="B154:B156"/>
-    <mergeCell ref="A154:A156"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>